<commit_message>
CE04OSSM added bar codes, hydgn sensors
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_CE04OSSM_00001.xlsx
+++ b/deployment/Omaha_Cal_Info_CE04OSSM_00001.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AST1799\Documents\OOI\OOI Douments\CI\asset-management\deployment\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="675" yWindow="555" windowWidth="12720" windowHeight="7185" tabRatio="766"/>
+    <workbookView xWindow="675" yWindow="555" windowWidth="12720" windowHeight="7185" tabRatio="766" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -19,12 +24,12 @@
     <definedName name="_FilterDatabase_0">[1]Moorings!#REF!</definedName>
     <definedName name="_FilterDatabase_0_0_0">[1]Moorings!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="177">
   <si>
     <t>Ref Des</t>
   </si>
@@ -323,12 +328,6 @@
     <t>CE04OSSM-RID27-04-DOSTAD000</t>
   </si>
   <si>
-    <t>CE04OSSM-RID27-07-NUTNRB000</t>
-  </si>
-  <si>
-    <t>CE04OSSM-RID27-08-SPKIRB000</t>
-  </si>
-  <si>
     <t>CE04OSSM-SBC11-00-CPMENG000</t>
   </si>
   <si>
@@ -528,6 +527,51 @@
   </si>
   <si>
     <t>N00735</t>
+  </si>
+  <si>
+    <t>CE04OSSM-SBD11-02-HYDGN0000</t>
+  </si>
+  <si>
+    <t>CE04OSSM-SBD12-03-HYDGN0000</t>
+  </si>
+  <si>
+    <t>CE04OSSM-RID26-07-NUTNRB000</t>
+  </si>
+  <si>
+    <t>CE04OSSM-RID26-08-SPKIRB000</t>
+  </si>
+  <si>
+    <t>CE04OSSM-00001+HYDGN1102</t>
+  </si>
+  <si>
+    <t>CE04OSSM-00001+HYDGN1203</t>
+  </si>
+  <si>
+    <t>OL000376</t>
+  </si>
+  <si>
+    <t>OL000377</t>
+  </si>
+  <si>
+    <t>OL000378</t>
+  </si>
+  <si>
+    <t>OL000379</t>
+  </si>
+  <si>
+    <t>OL000380</t>
+  </si>
+  <si>
+    <t>OL000381</t>
+  </si>
+  <si>
+    <t>OL000382</t>
+  </si>
+  <si>
+    <t>OL000383</t>
+  </si>
+  <si>
+    <t>OL000384</t>
   </si>
 </sst>
 </file>
@@ -1216,7 +1260,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1251,7 +1295,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1462,8 +1506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1487,7 +1531,7 @@
   <sheetData>
     <row r="1" spans="1:14" s="15" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>0</v>
@@ -1525,13 +1569,13 @@
     </row>
     <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D2" s="21">
         <v>1</v>
@@ -1546,16 +1590,16 @@
         <v>42499</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J2" s="5">
         <v>587</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="22">
@@ -1591,11 +1635,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I176"/>
+  <dimension ref="A1:P180"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5:E13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H124" sqref="H124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1612,12 +1656,12 @@
     <col min="10" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C1" s="29" t="s">
         <v>1</v>
@@ -1626,7 +1670,7 @@
         <v>34</v>
       </c>
       <c r="E1" s="29" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F1" s="29" t="s">
         <v>2</v>
@@ -1641,7 +1685,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1652,552 +1696,552 @@
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
     </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D3" s="9">
         <v>1</v>
       </c>
+      <c r="E3" t="s">
+        <v>168</v>
+      </c>
       <c r="F3" s="23" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
       <c r="I3" s="9" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B4"/>
       <c r="C4"/>
-      <c r="D4" s="9"/>
       <c r="F4" s="23"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-    </row>
-    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>89</v>
+    </row>
+    <row r="5" spans="1:16" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>162</v>
       </c>
       <c r="B5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D5" s="9">
         <v>1</v>
       </c>
       <c r="E5" t="s">
+        <v>169</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B6"/>
+      <c r="C6"/>
+      <c r="F6" s="23"/>
+    </row>
+    <row r="7" spans="1:16" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" s="9">
-        <v>44.366700000000002</v>
-      </c>
-      <c r="I5" s="23"/>
-    </row>
-    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B6" t="s">
-        <v>145</v>
-      </c>
-      <c r="C6" t="s">
-        <v>108</v>
-      </c>
-      <c r="D6" s="9">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
-        <v>163</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" s="9">
-        <v>-124.94451666666667</v>
-      </c>
-      <c r="I6" s="23"/>
-    </row>
-    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="B7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D7" s="9">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>163</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="H7" s="9">
-        <v>1.05</v>
-      </c>
-      <c r="I7" s="23"/>
-    </row>
-    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B8" t="s">
-        <v>145</v>
-      </c>
-      <c r="C8" t="s">
-        <v>108</v>
-      </c>
-      <c r="D8" s="9">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
-        <v>163</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="H8" s="9">
-        <v>4.08</v>
-      </c>
-      <c r="I8" s="23"/>
-    </row>
-    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="C8"/>
+      <c r="D8" s="9"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="P8" s="9"/>
+    </row>
+    <row r="9" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D9" s="9">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="H9" s="9">
-        <v>4.08</v>
+        <v>44.366700000000002</v>
       </c>
       <c r="I9" s="23"/>
-    </row>
-    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="L9" s="9"/>
+      <c r="P9" s="9"/>
+    </row>
+    <row r="10" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D10" s="9">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="H10" s="9">
-        <v>4.6399999999999997</v>
+        <v>-124.94451666666667</v>
       </c>
       <c r="I10" s="23"/>
-    </row>
-    <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="L10" s="9"/>
+      <c r="P10" s="9"/>
+    </row>
+    <row r="11" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B11" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D11" s="9">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="H11" s="9">
-        <v>1</v>
-      </c>
-      <c r="I11" s="9" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+        <v>1.05</v>
+      </c>
+      <c r="I11" s="23"/>
+      <c r="L11" s="9"/>
+      <c r="P11" s="9"/>
+    </row>
+    <row r="12" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B12" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D12" s="9">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H12" s="9">
-        <v>1</v>
-      </c>
-      <c r="I12" s="9" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+        <v>4.08</v>
+      </c>
+      <c r="I12" s="23"/>
+      <c r="L12" s="9"/>
+      <c r="P12" s="9"/>
+    </row>
+    <row r="13" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B13" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D13" s="9">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="H13" s="9">
-        <v>600</v>
-      </c>
-      <c r="I13" s="9" t="s">
+        <v>4.08</v>
+      </c>
+      <c r="I13" s="23"/>
+      <c r="L13" s="9"/>
+      <c r="P13" s="9"/>
+    </row>
+    <row r="14" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="C14"/>
-      <c r="D14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-    </row>
-    <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>106</v>
+      </c>
+      <c r="D14" s="9">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>161</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H14" s="9">
+        <v>4.6399999999999997</v>
+      </c>
+      <c r="I14" s="23"/>
+      <c r="L14" s="9"/>
+      <c r="P14" s="9"/>
+    </row>
+    <row r="15" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D15" s="9">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>149</v>
-      </c>
-      <c r="F15" s="30" t="s">
-        <v>148</v>
+        <v>161</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>160</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="H15" s="9">
-        <v>44.366700000000002</v>
-      </c>
-      <c r="I15" s="9"/>
-    </row>
-    <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="L15" s="9"/>
+      <c r="P15" s="9"/>
+    </row>
+    <row r="16" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B16" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C16" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D16" s="9">
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>149</v>
-      </c>
-      <c r="F16" s="30" t="s">
-        <v>148</v>
+        <v>161</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>160</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="H16" s="9">
-        <v>-124.94451666666667</v>
-      </c>
-      <c r="I16" s="9"/>
-    </row>
-    <row r="17" spans="1:9" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="C17"/>
-    </row>
-    <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B18" t="s">
-        <v>145</v>
-      </c>
-      <c r="C18" t="s">
-        <v>108</v>
-      </c>
-      <c r="D18" s="9">
         <v>1</v>
       </c>
-      <c r="E18" t="s">
-        <v>151</v>
-      </c>
-      <c r="F18" s="30" t="s">
-        <v>150</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="H18" s="9">
-        <v>44.366700000000002</v>
-      </c>
+      <c r="I16" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="L16" s="9"/>
+      <c r="P16" s="9"/>
+    </row>
+    <row r="17" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" t="s">
+        <v>143</v>
+      </c>
+      <c r="C17" t="s">
+        <v>106</v>
+      </c>
+      <c r="D17" s="9">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>161</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H17" s="9">
+        <v>600</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="L17" s="9"/>
+      <c r="P17" s="9"/>
+    </row>
+    <row r="18" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="C18"/>
+      <c r="D18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
       <c r="I18" s="9"/>
-    </row>
-    <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="L18" s="9"/>
+      <c r="P18" s="9"/>
+    </row>
+    <row r="19" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B19" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C19" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D19" s="9">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="F19" s="30" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="G19" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H19" s="9">
+        <v>44.366700000000002</v>
+      </c>
+      <c r="I19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="P19" s="9"/>
+    </row>
+    <row r="20" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B20" t="s">
+        <v>143</v>
+      </c>
+      <c r="C20" t="s">
+        <v>106</v>
+      </c>
+      <c r="D20" s="9">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>147</v>
+      </c>
+      <c r="F20" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="G20" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H19" s="9">
+      <c r="H20" s="9">
         <v>-124.94451666666667</v>
       </c>
-      <c r="I19" s="9"/>
-    </row>
-    <row r="20" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="C20"/>
-      <c r="D20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
       <c r="I20" s="9"/>
-    </row>
-    <row r="21" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B21" t="s">
-        <v>145</v>
-      </c>
-      <c r="C21" t="s">
-        <v>108</v>
-      </c>
-      <c r="D21" s="9">
+      <c r="L20" s="9"/>
+      <c r="P20" s="9"/>
+    </row>
+    <row r="21" spans="1:16" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="C21"/>
+    </row>
+    <row r="22" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B22" t="s">
+        <v>143</v>
+      </c>
+      <c r="C22" t="s">
+        <v>106</v>
+      </c>
+      <c r="D22" s="9">
         <v>1</v>
       </c>
-      <c r="E21" t="s">
-        <v>152</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="C22"/>
-      <c r="D22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
+      <c r="E22" t="s">
+        <v>149</v>
+      </c>
+      <c r="F22" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H22" s="9">
+        <v>44.366700000000002</v>
+      </c>
       <c r="I22" s="9"/>
-    </row>
-    <row r="23" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="L22" s="9"/>
+      <c r="P22" s="9"/>
+    </row>
+    <row r="23" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B23" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C23" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D23" s="9">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>153</v>
-      </c>
-      <c r="F23" s="9" t="s">
-        <v>113</v>
+        <v>149</v>
+      </c>
+      <c r="F23" s="30" t="s">
+        <v>148</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H23" s="9">
-        <v>44.366700000000002</v>
+        <v>-124.94451666666667</v>
       </c>
       <c r="I23" s="9"/>
-    </row>
-    <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B24" t="s">
-        <v>145</v>
-      </c>
-      <c r="C24" t="s">
-        <v>108</v>
-      </c>
-      <c r="D24" s="9">
+      <c r="L23" s="9"/>
+      <c r="P23" s="9"/>
+    </row>
+    <row r="24" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="C24"/>
+      <c r="D24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="P24" s="9"/>
+    </row>
+    <row r="25" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B25" t="s">
+        <v>143</v>
+      </c>
+      <c r="C25" t="s">
+        <v>106</v>
+      </c>
+      <c r="D25" s="9">
         <v>1</v>
       </c>
-      <c r="E24" t="s">
-        <v>153</v>
-      </c>
-      <c r="F24" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="H24" s="9">
-        <v>-124.94451666666667</v>
-      </c>
-      <c r="I24" s="9"/>
-    </row>
-    <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="C25"/>
-      <c r="D25" s="9"/>
-      <c r="F25" s="9"/>
+      <c r="E25" t="s">
+        <v>150</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>110</v>
+      </c>
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
-    </row>
-    <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B26" t="s">
-        <v>145</v>
-      </c>
-      <c r="C26" t="s">
-        <v>108</v>
-      </c>
-      <c r="D26" s="9">
-        <v>1</v>
-      </c>
-      <c r="E26" t="s">
-        <v>154</v>
-      </c>
-      <c r="F26" s="9">
-        <v>19002</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H26" s="9">
-        <v>5000</v>
-      </c>
+      <c r="I25" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="L25" s="9"/>
+      <c r="P25" s="9"/>
+    </row>
+    <row r="26" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="C26"/>
+      <c r="D26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
       <c r="I26" s="9"/>
-    </row>
-    <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="L26" s="9"/>
+      <c r="P26" s="9"/>
+    </row>
+    <row r="27" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="B27" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C27" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D27" s="9">
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>154</v>
-      </c>
-      <c r="F27" s="9">
-        <v>19002</v>
+        <v>151</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>111</v>
       </c>
       <c r="G27" s="9" t="s">
         <v>5</v>
@@ -2206,25 +2250,27 @@
         <v>44.366700000000002</v>
       </c>
       <c r="I27" s="9"/>
-    </row>
-    <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="L27" s="9"/>
+      <c r="P27" s="9"/>
+    </row>
+    <row r="28" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="B28" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C28" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D28" s="9">
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>154</v>
-      </c>
-      <c r="F28" s="9">
-        <v>19002</v>
+        <v>151</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>111</v>
       </c>
       <c r="G28" s="9" t="s">
         <v>6</v>
@@ -2233,2037 +2279,2197 @@
         <v>-124.94451666666667</v>
       </c>
       <c r="I28" s="9"/>
-    </row>
-    <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B29" t="s">
-        <v>145</v>
-      </c>
-      <c r="C29" t="s">
-        <v>108</v>
-      </c>
-      <c r="D29" s="9">
-        <v>1</v>
-      </c>
-      <c r="E29" t="s">
-        <v>154</v>
-      </c>
-      <c r="F29" s="9">
-        <v>19002</v>
-      </c>
-      <c r="G29" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="H29" s="9">
-        <v>0.45</v>
-      </c>
+      <c r="L28" s="9"/>
+      <c r="P28" s="9"/>
+    </row>
+    <row r="29" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="C29"/>
+      <c r="D29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
       <c r="I29" s="9"/>
-    </row>
-    <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="L29" s="9"/>
+    </row>
+    <row r="30" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B30" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C30" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D30" s="9">
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F30" s="9">
         <v>19002</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H30" s="9">
-        <v>0.45</v>
+        <v>5000</v>
       </c>
       <c r="I30" s="9"/>
-    </row>
-    <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="L30" s="9"/>
+    </row>
+    <row r="31" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B31" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C31" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D31" s="9">
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F31" s="9">
         <v>19002</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="H31" s="9">
-        <v>0.45</v>
+        <v>44.366700000000002</v>
       </c>
       <c r="I31" s="9"/>
-    </row>
-    <row r="32" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="L31" s="9"/>
+    </row>
+    <row r="32" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B32" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C32" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D32" s="9">
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F32" s="9">
         <v>19002</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="H32" s="9">
+        <v>-124.94451666666667</v>
+      </c>
+      <c r="I32" s="9"/>
+      <c r="L32" s="9"/>
+    </row>
+    <row r="33" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B33" t="s">
+        <v>143</v>
+      </c>
+      <c r="C33" t="s">
+        <v>106</v>
+      </c>
+      <c r="D33" s="9">
+        <v>1</v>
+      </c>
+      <c r="E33" t="s">
+        <v>152</v>
+      </c>
+      <c r="F33" s="9">
+        <v>19002</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H33" s="9">
         <v>0.45</v>
       </c>
-      <c r="I32" s="9"/>
-    </row>
-    <row r="33" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="C33"/>
-      <c r="D33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
       <c r="I33" s="9"/>
-    </row>
-    <row r="34" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="L33" s="9"/>
+    </row>
+    <row r="34" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="B34" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C34" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D34" s="9">
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>155</v>
-      </c>
-      <c r="F34" s="9" t="s">
-        <v>116</v>
+        <v>152</v>
+      </c>
+      <c r="F34" s="9">
+        <v>19002</v>
       </c>
       <c r="G34" s="9" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H34" s="9">
-        <v>17533</v>
+        <v>0.45</v>
       </c>
       <c r="I34" s="9"/>
-    </row>
-    <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="L34" s="9"/>
+    </row>
+    <row r="35" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="B35" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C35" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D35" s="9">
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>155</v>
-      </c>
-      <c r="F35" s="9" t="s">
-        <v>116</v>
+        <v>152</v>
+      </c>
+      <c r="F35" s="9">
+        <v>19002</v>
       </c>
       <c r="G35" s="9" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="H35" s="9">
-        <v>101</v>
+        <v>0.45</v>
       </c>
       <c r="I35" s="9"/>
-    </row>
-    <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="L35" s="9"/>
+    </row>
+    <row r="36" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="B36" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C36" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D36" s="9">
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>155</v>
-      </c>
-      <c r="F36" s="9" t="s">
-        <v>116</v>
+        <v>152</v>
+      </c>
+      <c r="F36" s="9">
+        <v>19002</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="H36" s="9">
-        <v>2229</v>
+        <v>0.45</v>
       </c>
       <c r="I36" s="9"/>
-    </row>
-    <row r="37" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B37" t="s">
-        <v>145</v>
-      </c>
-      <c r="C37" t="s">
-        <v>108</v>
-      </c>
-      <c r="D37" s="9">
-        <v>1</v>
-      </c>
-      <c r="E37" t="s">
-        <v>155</v>
-      </c>
-      <c r="F37" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="G37" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H37" s="9">
-        <v>38502</v>
-      </c>
+      <c r="L36" s="9"/>
+    </row>
+    <row r="37" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="C37"/>
+      <c r="D37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
       <c r="I37" s="9"/>
-    </row>
-    <row r="38" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="L37" s="9"/>
+    </row>
+    <row r="38" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B38" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C38" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D38" s="9">
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G38" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H38" s="28">
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="H38" s="9">
+        <v>17533</v>
       </c>
       <c r="I38" s="9"/>
-    </row>
-    <row r="39" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="L38" s="9"/>
+    </row>
+    <row r="39" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B39" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C39" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D39" s="9">
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G39" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H39" s="28">
-        <v>1</v>
+        <v>16</v>
+      </c>
+      <c r="H39" s="9">
+        <v>101</v>
       </c>
       <c r="I39" s="9"/>
-    </row>
-    <row r="40" spans="1:9" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="9" t="s">
+      <c r="L39" s="9"/>
+    </row>
+    <row r="40" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B40" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C40" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D40" s="9">
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G40" s="9" t="s">
-        <v>76</v>
+        <v>15</v>
       </c>
       <c r="H40" s="9">
-        <v>35</v>
-      </c>
-      <c r="I40" s="9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="C41"/>
-      <c r="D41" s="9"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="9"/>
-      <c r="H41" s="9"/>
+        <v>2229</v>
+      </c>
+      <c r="I40" s="9"/>
+      <c r="L40" s="9"/>
+    </row>
+    <row r="41" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B41" t="s">
+        <v>143</v>
+      </c>
+      <c r="C41" t="s">
+        <v>106</v>
+      </c>
+      <c r="D41" s="9">
+        <v>1</v>
+      </c>
+      <c r="E41" t="s">
+        <v>153</v>
+      </c>
+      <c r="F41" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H41" s="9">
+        <v>38502</v>
+      </c>
       <c r="I41" s="9"/>
-    </row>
-    <row r="42" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="L41" s="9"/>
+    </row>
+    <row r="42" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B42" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C42" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D42" s="9">
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G42" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="H42" s="9" t="s">
-        <v>120</v>
+        <v>19</v>
+      </c>
+      <c r="H42" s="28">
+        <v>0</v>
       </c>
       <c r="I42" s="9"/>
-    </row>
-    <row r="43" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="L42" s="9"/>
+    </row>
+    <row r="43" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B43" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C43" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D43" s="9">
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="H43" s="9" t="s">
-        <v>121</v>
+        <v>18</v>
+      </c>
+      <c r="H43" s="28">
+        <v>1</v>
       </c>
       <c r="I43" s="9"/>
-    </row>
-    <row r="44" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>95</v>
+      <c r="L43" s="9"/>
+    </row>
+    <row r="44" spans="1:12" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A44" s="9" t="s">
+        <v>94</v>
       </c>
       <c r="B44" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C44" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D44" s="9">
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F44" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G44" s="9" t="s">
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="H44" s="9">
-        <v>19.899999999999999</v>
-      </c>
-      <c r="I44" s="9"/>
-    </row>
-    <row r="45" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B45" t="s">
-        <v>145</v>
-      </c>
-      <c r="C45" t="s">
-        <v>108</v>
-      </c>
-      <c r="D45" s="9">
-        <v>1</v>
-      </c>
-      <c r="E45" t="s">
-        <v>156</v>
-      </c>
-      <c r="F45" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="G45" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="H45" s="9" t="s">
-        <v>122</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="I44" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="C45"/>
+      <c r="D45" s="9"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="9"/>
+      <c r="H45" s="9"/>
       <c r="I45" s="9"/>
-    </row>
-    <row r="46" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="L45" s="9"/>
+    </row>
+    <row r="46" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>95</v>
       </c>
       <c r="B46" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C46" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D46" s="9">
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G46" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H46" s="9" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="I46" s="9"/>
-    </row>
-    <row r="47" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="L46" s="9"/>
+    </row>
+    <row r="47" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>95</v>
       </c>
       <c r="B47" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C47" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D47" s="9">
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F47" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G47" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H47" s="9" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="I47" s="9"/>
-    </row>
-    <row r="48" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="L47" s="9"/>
+    </row>
+    <row r="48" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>95</v>
       </c>
       <c r="B48" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C48" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D48" s="9">
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F48" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G48" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="H48" s="9" t="s">
-        <v>118</v>
+        <v>42</v>
+      </c>
+      <c r="H48" s="9">
+        <v>19.899999999999999</v>
       </c>
       <c r="I48" s="9"/>
-    </row>
-    <row r="49" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A49" s="6" t="s">
+      <c r="L48" s="9"/>
+    </row>
+    <row r="49" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>95</v>
       </c>
       <c r="B49" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C49" t="s">
-        <v>108</v>
-      </c>
-      <c r="D49" s="6">
+        <v>106</v>
+      </c>
+      <c r="D49" s="9">
         <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>156</v>
-      </c>
-      <c r="F49" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="G49" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="H49" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="C50"/>
-      <c r="D50" s="9"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="9"/>
-      <c r="H50" s="9"/>
+        <v>154</v>
+      </c>
+      <c r="F49" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="G49" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H49" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="I49" s="9"/>
+      <c r="L49" s="9"/>
+    </row>
+    <row r="50" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B50" t="s">
+        <v>143</v>
+      </c>
+      <c r="C50" t="s">
+        <v>106</v>
+      </c>
+      <c r="D50" s="9">
+        <v>1</v>
+      </c>
+      <c r="E50" t="s">
+        <v>154</v>
+      </c>
+      <c r="F50" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="G50" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="H50" s="9" t="s">
+        <v>121</v>
+      </c>
       <c r="I50" s="9"/>
-    </row>
-    <row r="51" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="L50" s="9"/>
+    </row>
+    <row r="51" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B51" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C51" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D51" s="9">
         <v>1</v>
       </c>
       <c r="E51" t="s">
-        <v>157</v>
-      </c>
-      <c r="F51" s="9">
-        <v>1151</v>
+        <v>154</v>
+      </c>
+      <c r="F51" s="9" t="s">
+        <v>113</v>
       </c>
       <c r="G51" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H51" s="9">
-        <v>53</v>
+        <v>80</v>
+      </c>
+      <c r="H51" s="9" t="s">
+        <v>122</v>
       </c>
       <c r="I51" s="9"/>
-    </row>
-    <row r="52" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="L51" s="9"/>
+    </row>
+    <row r="52" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B52" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C52" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D52" s="9">
         <v>1</v>
       </c>
       <c r="E52" t="s">
-        <v>157</v>
-      </c>
-      <c r="F52" s="9">
-        <v>1151</v>
+        <v>154</v>
+      </c>
+      <c r="F52" s="9" t="s">
+        <v>113</v>
       </c>
       <c r="G52" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="H52" s="9">
-        <v>1.877E-6</v>
+        <v>81</v>
+      </c>
+      <c r="H52" s="9" t="s">
+        <v>116</v>
       </c>
       <c r="I52" s="9"/>
-    </row>
-    <row r="53" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>96</v>
+      <c r="L52" s="9"/>
+    </row>
+    <row r="53" spans="1:12" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A53" s="6" t="s">
+        <v>95</v>
       </c>
       <c r="B53" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C53" t="s">
-        <v>108</v>
-      </c>
-      <c r="D53" s="9">
+        <v>106</v>
+      </c>
+      <c r="D53" s="6">
         <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>157</v>
-      </c>
-      <c r="F53" s="9">
-        <v>1151</v>
-      </c>
-      <c r="G53" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H53" s="9">
-        <v>48</v>
-      </c>
-      <c r="I53" s="9"/>
-    </row>
-    <row r="54" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B54" t="s">
-        <v>145</v>
-      </c>
-      <c r="C54" t="s">
-        <v>108</v>
-      </c>
-      <c r="D54" s="9">
-        <v>1</v>
-      </c>
-      <c r="E54" t="s">
-        <v>157</v>
-      </c>
-      <c r="F54" s="9">
-        <v>1151</v>
-      </c>
-      <c r="G54" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="H54" s="9">
-        <v>7.3000000000000001E-3</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="G53" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="H53" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="L53" s="9"/>
+    </row>
+    <row r="54" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="C54"/>
+      <c r="D54" s="9"/>
+      <c r="F54" s="9"/>
+      <c r="G54" s="9"/>
+      <c r="H54" s="9"/>
       <c r="I54" s="9"/>
-    </row>
-    <row r="55" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="L54" s="9"/>
+    </row>
+    <row r="55" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B55" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C55" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D55" s="9">
         <v>1</v>
       </c>
       <c r="E55" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F55" s="9">
         <v>1151</v>
       </c>
       <c r="G55" s="9" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="H55" s="9">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="I55" s="9"/>
-    </row>
-    <row r="56" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="L55" s="9"/>
+    </row>
+    <row r="56" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B56" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C56" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D56" s="9">
         <v>1</v>
       </c>
       <c r="E56" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F56" s="9">
         <v>1151</v>
       </c>
       <c r="G56" s="9" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="H56" s="9">
-        <v>9.0200000000000002E-2</v>
+        <v>1.877E-6</v>
       </c>
       <c r="I56" s="9"/>
-    </row>
-    <row r="57" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="L56" s="9"/>
+    </row>
+    <row r="57" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B57" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C57" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D57" s="9">
         <v>1</v>
       </c>
       <c r="E57" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F57" s="9">
         <v>1151</v>
       </c>
       <c r="G57" s="9" t="s">
-        <v>83</v>
+        <v>9</v>
       </c>
       <c r="H57" s="9">
-        <v>117</v>
-      </c>
-      <c r="I57" s="9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="I57" s="9"/>
+      <c r="L57" s="9"/>
+    </row>
+    <row r="58" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B58" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C58" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D58" s="9">
         <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F58" s="9">
         <v>1151</v>
       </c>
       <c r="G58" s="9" t="s">
-        <v>84</v>
+        <v>10</v>
       </c>
       <c r="H58" s="9">
-        <v>700</v>
-      </c>
-      <c r="I58" s="9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+        <v>7.3000000000000001E-3</v>
+      </c>
+      <c r="I58" s="9"/>
+      <c r="L58" s="9"/>
+    </row>
+    <row r="59" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B59" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C59" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D59" s="9">
         <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F59" s="9">
         <v>1151</v>
       </c>
       <c r="G59" s="9" t="s">
-        <v>85</v>
+        <v>13</v>
       </c>
       <c r="H59" s="9">
-        <v>1.08</v>
-      </c>
-      <c r="I59" s="9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="I59" s="9"/>
+      <c r="L59" s="9"/>
+    </row>
+    <row r="60" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B60" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C60" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D60" s="9">
         <v>1</v>
       </c>
       <c r="E60" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F60" s="9">
         <v>1151</v>
       </c>
       <c r="G60" s="9" t="s">
-        <v>86</v>
+        <v>12</v>
       </c>
       <c r="H60" s="9">
-        <v>3.9E-2</v>
-      </c>
-      <c r="I60" s="9" t="s">
+        <v>9.0200000000000002E-2</v>
+      </c>
+      <c r="I60" s="9"/>
+      <c r="L60" s="9"/>
+    </row>
+    <row r="61" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B61" t="s">
+        <v>143</v>
+      </c>
+      <c r="C61" t="s">
+        <v>106</v>
+      </c>
+      <c r="D61" s="9">
+        <v>1</v>
+      </c>
+      <c r="E61" t="s">
+        <v>155</v>
+      </c>
+      <c r="F61" s="9">
+        <v>1151</v>
+      </c>
+      <c r="G61" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="H61" s="9">
+        <v>117</v>
+      </c>
+      <c r="I61" s="9" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="C61"/>
-      <c r="D61" s="9"/>
-      <c r="F61" s="9"/>
-      <c r="G61" s="9"/>
-      <c r="H61" s="9"/>
-      <c r="I61" s="9"/>
-    </row>
-    <row r="62" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="L61" s="9"/>
+    </row>
+    <row r="62" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B62" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C62" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D62" s="9">
         <v>1</v>
       </c>
       <c r="E62" t="s">
-        <v>158</v>
-      </c>
-      <c r="F62" s="9" t="s">
-        <v>114</v>
+        <v>155</v>
+      </c>
+      <c r="F62" s="9">
+        <v>1151</v>
       </c>
       <c r="G62" s="9" t="s">
-        <v>5</v>
+        <v>84</v>
       </c>
       <c r="H62" s="9">
-        <v>44.366700000000002</v>
-      </c>
-      <c r="I62" s="9"/>
-    </row>
-    <row r="63" spans="1:9" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A63" s="7" t="s">
-        <v>97</v>
+        <v>700</v>
+      </c>
+      <c r="I62" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="L62" s="9"/>
+    </row>
+    <row r="63" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>96</v>
       </c>
       <c r="B63" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C63" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D63" s="9">
         <v>1</v>
       </c>
       <c r="E63" t="s">
-        <v>158</v>
-      </c>
-      <c r="F63" s="9" t="s">
-        <v>114</v>
+        <v>155</v>
+      </c>
+      <c r="F63" s="9">
+        <v>1151</v>
       </c>
       <c r="G63" s="9" t="s">
-        <v>6</v>
+        <v>85</v>
       </c>
       <c r="H63" s="9">
-        <v>-124.94451666666667</v>
-      </c>
-      <c r="I63" s="9"/>
-    </row>
-    <row r="64" spans="1:9" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A64" s="7" t="s">
-        <v>97</v>
+        <v>1.08</v>
+      </c>
+      <c r="I63" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="L63" s="9"/>
+    </row>
+    <row r="64" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>96</v>
       </c>
       <c r="B64" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C64" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D64" s="9">
         <v>1</v>
       </c>
       <c r="E64" t="s">
-        <v>158</v>
-      </c>
-      <c r="F64" s="9" t="s">
-        <v>114</v>
+        <v>155</v>
+      </c>
+      <c r="F64" s="9">
+        <v>1151</v>
       </c>
       <c r="G64" s="9" t="s">
-        <v>54</v>
+        <v>86</v>
       </c>
       <c r="H64" s="9">
-        <v>1.254062E-3</v>
-      </c>
-      <c r="I64" s="9"/>
-    </row>
-    <row r="65" spans="1:9" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A65" s="7" t="s">
+        <v>3.9E-2</v>
+      </c>
+      <c r="I64" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="L64" s="9"/>
+    </row>
+    <row r="65" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="C65"/>
+      <c r="D65" s="9"/>
+      <c r="F65" s="9"/>
+      <c r="G65" s="9"/>
+      <c r="H65" s="9"/>
+      <c r="I65" s="9"/>
+      <c r="L65" s="9"/>
+    </row>
+    <row r="66" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B65" t="s">
-        <v>145</v>
-      </c>
-      <c r="C65" t="s">
-        <v>108</v>
-      </c>
-      <c r="D65" s="9">
-        <v>1</v>
-      </c>
-      <c r="E65" t="s">
-        <v>158</v>
-      </c>
-      <c r="F65" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="G65" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="H65" s="9">
-        <v>2.7485969999999999E-4</v>
-      </c>
-      <c r="I65" s="9"/>
-    </row>
-    <row r="66" spans="1:9" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A66" s="7" t="s">
-        <v>97</v>
-      </c>
       <c r="B66" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C66" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D66" s="9">
         <v>1</v>
       </c>
       <c r="E66" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F66" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G66" s="9" t="s">
-        <v>56</v>
+        <v>5</v>
       </c>
       <c r="H66" s="9">
-        <v>-1.176268E-6</v>
+        <v>44.366700000000002</v>
       </c>
       <c r="I66" s="9"/>
-    </row>
-    <row r="67" spans="1:9" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="L66" s="9"/>
+    </row>
+    <row r="67" spans="1:12" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
         <v>97</v>
       </c>
       <c r="B67" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C67" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D67" s="9">
         <v>1</v>
       </c>
       <c r="E67" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F67" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G67" s="9" t="s">
-        <v>57</v>
+        <v>6</v>
       </c>
       <c r="H67" s="9">
-        <v>1.8403809999999999E-7</v>
+        <v>-124.94451666666667</v>
       </c>
       <c r="I67" s="9"/>
-    </row>
-    <row r="68" spans="1:9" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="L67" s="9"/>
+    </row>
+    <row r="68" spans="1:12" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
         <v>97</v>
       </c>
       <c r="B68" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C68" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D68" s="9">
         <v>1</v>
       </c>
       <c r="E68" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F68" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G68" s="9" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="H68" s="9">
-        <v>-59.278405200000002</v>
+        <v>1.254062E-3</v>
       </c>
       <c r="I68" s="9"/>
-    </row>
-    <row r="69" spans="1:9" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="L68" s="9"/>
+    </row>
+    <row r="69" spans="1:12" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
         <v>97</v>
       </c>
       <c r="B69" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C69" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D69" s="9">
         <v>1</v>
       </c>
       <c r="E69" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F69" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G69" s="9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H69" s="9">
-        <v>53.6581701</v>
+        <v>2.7485969999999999E-4</v>
       </c>
       <c r="I69" s="9"/>
-    </row>
-    <row r="70" spans="1:9" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="L69" s="9"/>
+    </row>
+    <row r="70" spans="1:12" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
         <v>97</v>
       </c>
       <c r="B70" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C70" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D70" s="9">
         <v>1</v>
       </c>
       <c r="E70" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F70" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G70" s="9" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H70" s="9">
-        <v>-0.35581304499999999</v>
+        <v>-1.176268E-6</v>
       </c>
       <c r="I70" s="9"/>
-    </row>
-    <row r="71" spans="1:9" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="L70" s="9"/>
+    </row>
+    <row r="71" spans="1:12" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
         <v>97</v>
       </c>
       <c r="B71" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C71" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D71" s="9">
         <v>1</v>
       </c>
       <c r="E71" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F71" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G71" s="9" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H71" s="9">
-        <v>524875.41099999996</v>
+        <v>1.8403809999999999E-7</v>
       </c>
       <c r="I71" s="9"/>
-    </row>
-    <row r="72" spans="1:9" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="L71" s="9"/>
+    </row>
+    <row r="72" spans="1:12" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
         <v>97</v>
       </c>
       <c r="B72" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C72" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D72" s="9">
         <v>1</v>
       </c>
       <c r="E72" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F72" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G72" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H72" s="9">
-        <v>-18.321615300000001</v>
+        <v>-59.278405200000002</v>
       </c>
       <c r="I72" s="9"/>
-    </row>
-    <row r="73" spans="1:9" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="L72" s="9"/>
+    </row>
+    <row r="73" spans="1:12" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
         <v>97</v>
       </c>
       <c r="B73" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C73" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D73" s="9">
         <v>1</v>
       </c>
       <c r="E73" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F73" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G73" s="9" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H73" s="9">
-        <v>0.179273715</v>
+        <v>53.6581701</v>
       </c>
       <c r="I73" s="9"/>
-    </row>
-    <row r="74" spans="1:9" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="L73" s="9"/>
+    </row>
+    <row r="74" spans="1:12" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
         <v>97</v>
       </c>
       <c r="B74" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C74" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D74" s="9">
         <v>1</v>
       </c>
       <c r="E74" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F74" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G74" s="9" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H74" s="9">
-        <v>25.100625000000001</v>
+        <v>-0.35581304499999999</v>
       </c>
       <c r="I74" s="9"/>
-    </row>
-    <row r="75" spans="1:9" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="L74" s="9"/>
+    </row>
+    <row r="75" spans="1:12" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
         <v>97</v>
       </c>
       <c r="B75" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C75" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D75" s="9">
         <v>1</v>
       </c>
       <c r="E75" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F75" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G75" s="9" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="H75" s="9">
-        <v>3.2499999999999999E-4</v>
+        <v>524875.41099999996</v>
       </c>
       <c r="I75" s="9"/>
-    </row>
-    <row r="76" spans="1:9" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="L75" s="9"/>
+    </row>
+    <row r="76" spans="1:12" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
         <v>97</v>
       </c>
       <c r="B76" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C76" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D76" s="9">
         <v>1</v>
       </c>
       <c r="E76" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F76" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G76" s="9" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="H76" s="9">
-        <v>0</v>
+        <v>-18.321615300000001</v>
       </c>
       <c r="I76" s="9"/>
-    </row>
-    <row r="77" spans="1:9" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="L76" s="9"/>
+    </row>
+    <row r="77" spans="1:12" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
         <v>97</v>
       </c>
       <c r="B77" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C77" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D77" s="9">
         <v>1</v>
       </c>
       <c r="E77" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F77" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G77" s="9" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H77" s="9">
-        <v>-0.146232899</v>
+        <v>0.179273715</v>
       </c>
       <c r="I77" s="9"/>
-    </row>
-    <row r="78" spans="1:9" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="L77" s="9"/>
+    </row>
+    <row r="78" spans="1:12" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
         <v>97</v>
       </c>
       <c r="B78" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C78" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D78" s="9">
         <v>1</v>
       </c>
       <c r="E78" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F78" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G78" s="9" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H78" s="9">
-        <v>4.8715891399999999E-4</v>
+        <v>25.100625000000001</v>
       </c>
       <c r="I78" s="9"/>
-    </row>
-    <row r="79" spans="1:9" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="L78" s="9"/>
+    </row>
+    <row r="79" spans="1:12" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
         <v>97</v>
       </c>
       <c r="B79" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C79" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D79" s="9">
         <v>1</v>
       </c>
       <c r="E79" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F79" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G79" s="9" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="H79" s="9">
-        <v>-5.9564635300000001E-12</v>
+        <v>3.2499999999999999E-4</v>
       </c>
       <c r="I79" s="9"/>
-    </row>
-    <row r="80" spans="1:9" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="L79" s="9"/>
+    </row>
+    <row r="80" spans="1:12" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
         <v>97</v>
       </c>
       <c r="B80" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C80" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D80" s="9">
         <v>1</v>
       </c>
       <c r="E80" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F80" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G80" s="9" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H80" s="9">
-        <v>-0.97940059999999995</v>
+        <v>0</v>
       </c>
       <c r="I80" s="9"/>
-    </row>
-    <row r="81" spans="1:9" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="L80" s="9"/>
+    </row>
+    <row r="81" spans="1:12" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>97</v>
       </c>
       <c r="B81" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C81" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D81" s="9">
         <v>1</v>
       </c>
       <c r="E81" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F81" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G81" s="9" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H81" s="9">
-        <v>0.13973099999999999</v>
+        <v>-0.146232899</v>
       </c>
       <c r="I81" s="9"/>
-    </row>
-    <row r="82" spans="1:9" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="L81" s="9"/>
+    </row>
+    <row r="82" spans="1:12" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
         <v>97</v>
       </c>
       <c r="B82" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C82" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D82" s="9">
         <v>1</v>
       </c>
       <c r="E82" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F82" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G82" s="9" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H82" s="9">
-        <v>-2.6729169999999998E-4</v>
+        <v>4.8715891399999999E-4</v>
       </c>
       <c r="I82" s="9"/>
-    </row>
-    <row r="83" spans="1:9" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="L82" s="9"/>
+    </row>
+    <row r="83" spans="1:12" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
         <v>97</v>
       </c>
       <c r="B83" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C83" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D83" s="9">
         <v>1</v>
       </c>
       <c r="E83" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F83" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G83" s="9" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H83" s="9">
-        <v>4.0018580000000002E-5</v>
+        <v>-5.9564635300000001E-12</v>
       </c>
       <c r="I83" s="9"/>
-    </row>
-    <row r="84" spans="1:9" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="L83" s="9"/>
+    </row>
+    <row r="84" spans="1:12" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
         <v>97</v>
       </c>
       <c r="B84" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C84" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D84" s="9">
         <v>1</v>
       </c>
       <c r="E84" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F84" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G84" s="9" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H84" s="9">
-        <v>-9.5700000000000003E-8</v>
+        <v>-0.97940059999999995</v>
       </c>
       <c r="I84" s="9"/>
-    </row>
-    <row r="85" spans="1:9" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="L84" s="9"/>
+    </row>
+    <row r="85" spans="1:12" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
         <v>97</v>
       </c>
       <c r="B85" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C85" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D85" s="9">
         <v>1</v>
       </c>
       <c r="E85" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F85" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G85" s="9" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="H85" s="9">
-        <v>3.2499999999999998E-6</v>
+        <v>0.13973099999999999</v>
       </c>
       <c r="I85" s="9"/>
-    </row>
-    <row r="86" spans="1:9" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="C86"/>
-    </row>
-    <row r="87" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
-        <v>98</v>
+      <c r="L85" s="9"/>
+    </row>
+    <row r="86" spans="1:12" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A86" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B86" t="s">
+        <v>143</v>
+      </c>
+      <c r="C86" t="s">
+        <v>106</v>
+      </c>
+      <c r="D86" s="9">
+        <v>1</v>
+      </c>
+      <c r="E86" t="s">
+        <v>156</v>
+      </c>
+      <c r="F86" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="G86" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H86" s="9">
+        <v>-2.6729169999999998E-4</v>
+      </c>
+      <c r="I86" s="9"/>
+      <c r="L86" s="9"/>
+    </row>
+    <row r="87" spans="1:12" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A87" s="7" t="s">
+        <v>97</v>
       </c>
       <c r="B87" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C87" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D87" s="9">
         <v>1</v>
       </c>
       <c r="E87" t="s">
-        <v>159</v>
-      </c>
-      <c r="F87" s="9">
-        <v>291</v>
+        <v>156</v>
+      </c>
+      <c r="F87" s="9" t="s">
+        <v>112</v>
       </c>
       <c r="G87" s="9" t="s">
-        <v>5</v>
+        <v>73</v>
       </c>
       <c r="H87" s="9">
-        <v>44.366700000000002</v>
+        <v>4.0018580000000002E-5</v>
       </c>
       <c r="I87" s="9"/>
-    </row>
-    <row r="88" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
-        <v>98</v>
+      <c r="L87" s="9"/>
+    </row>
+    <row r="88" spans="1:12" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A88" s="7" t="s">
+        <v>97</v>
       </c>
       <c r="B88" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C88" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D88" s="9">
         <v>1</v>
       </c>
       <c r="E88" t="s">
-        <v>159</v>
-      </c>
-      <c r="F88" s="9">
-        <v>291</v>
+        <v>156</v>
+      </c>
+      <c r="F88" s="9" t="s">
+        <v>112</v>
       </c>
       <c r="G88" s="9" t="s">
-        <v>6</v>
+        <v>74</v>
       </c>
       <c r="H88" s="9">
-        <v>-124.94451666666667</v>
+        <v>-9.5700000000000003E-8</v>
       </c>
       <c r="I88" s="9"/>
-    </row>
-    <row r="89" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
-        <v>98</v>
+      <c r="L88" s="9"/>
+    </row>
+    <row r="89" spans="1:12" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A89" s="7" t="s">
+        <v>97</v>
       </c>
       <c r="B89" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C89" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D89" s="9">
         <v>1</v>
       </c>
       <c r="E89" t="s">
-        <v>159</v>
-      </c>
-      <c r="F89" s="9">
-        <v>291</v>
+        <v>156</v>
+      </c>
+      <c r="F89" s="9" t="s">
+        <v>112</v>
       </c>
       <c r="G89" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H89" s="9" t="s">
-        <v>125</v>
+        <v>75</v>
+      </c>
+      <c r="H89" s="9">
+        <v>3.2499999999999998E-6</v>
       </c>
       <c r="I89" s="9"/>
-    </row>
-    <row r="90" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="L89" s="9"/>
+    </row>
+    <row r="90" spans="1:12" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="C90"/>
-      <c r="D90" s="9"/>
-      <c r="F90" s="9"/>
-      <c r="G90" s="9"/>
-      <c r="H90" s="9"/>
-      <c r="I90" s="9"/>
-    </row>
-    <row r="91" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="91" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B91" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C91" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D91" s="9">
         <v>1</v>
       </c>
       <c r="E91" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F91" s="9">
-        <v>256</v>
+        <v>291</v>
       </c>
       <c r="G91" s="9" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="H91" s="9">
-        <v>217</v>
-      </c>
-      <c r="I91" s="9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+        <v>44.366700000000002</v>
+      </c>
+      <c r="I91" s="9"/>
+      <c r="L91" s="9"/>
+    </row>
+    <row r="92" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B92" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C92" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D92" s="9">
         <v>1</v>
       </c>
       <c r="E92" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F92" s="9">
-        <v>256</v>
+        <v>291</v>
       </c>
       <c r="G92" s="9" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="H92" s="9">
-        <v>240</v>
-      </c>
-      <c r="I92" s="9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+        <v>-124.94451666666667</v>
+      </c>
+      <c r="I92" s="9"/>
+      <c r="L92" s="9"/>
+    </row>
+    <row r="93" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B93" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C93" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D93" s="9">
         <v>1</v>
       </c>
       <c r="E93" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F93" s="9">
-        <v>256</v>
+        <v>291</v>
       </c>
       <c r="G93" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="H93" s="9">
-        <v>20.035643160334502</v>
+        <v>11</v>
+      </c>
+      <c r="H93" s="9" t="s">
+        <v>123</v>
       </c>
       <c r="I93" s="9"/>
-    </row>
-    <row r="94" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B94" t="s">
-        <v>145</v>
-      </c>
-      <c r="C94" t="s">
-        <v>108</v>
-      </c>
-      <c r="D94" s="9">
-        <v>1</v>
-      </c>
-      <c r="E94" t="s">
-        <v>160</v>
-      </c>
-      <c r="F94" s="9">
-        <v>256</v>
-      </c>
-      <c r="G94" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H94" s="27" t="s">
-        <v>142</v>
-      </c>
+      <c r="L93" s="9"/>
+    </row>
+    <row r="94" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="C94"/>
+      <c r="D94" s="9"/>
+      <c r="F94" s="9"/>
+      <c r="G94" s="9"/>
+      <c r="H94" s="9"/>
       <c r="I94" s="9"/>
-    </row>
-    <row r="95" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="L94" s="9"/>
+    </row>
+    <row r="95" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>99</v>
+        <v>164</v>
       </c>
       <c r="B95" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C95" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D95" s="9">
         <v>1</v>
       </c>
       <c r="E95" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F95" s="9">
         <v>256</v>
       </c>
       <c r="G95" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="H95" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="I95" s="9"/>
-    </row>
-    <row r="96" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
-        <v>99</v>
+        <v>44</v>
+      </c>
+      <c r="H95" s="9">
+        <v>217</v>
+      </c>
+      <c r="I95" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="L95" s="9"/>
+    </row>
+    <row r="96" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A96" s="9" t="s">
+        <v>164</v>
       </c>
       <c r="B96" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C96" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D96" s="9">
         <v>1</v>
       </c>
       <c r="E96" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F96" s="9">
         <v>256</v>
       </c>
       <c r="G96" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H96" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="I96" s="9"/>
-    </row>
-    <row r="97" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
-        <v>99</v>
+        <v>45</v>
+      </c>
+      <c r="H96" s="9">
+        <v>240</v>
+      </c>
+      <c r="I96" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="L96" s="9"/>
+    </row>
+    <row r="97" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A97" s="9" t="s">
+        <v>164</v>
       </c>
       <c r="B97" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C97" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D97" s="9">
         <v>1</v>
       </c>
       <c r="E97" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F97" s="9">
         <v>256</v>
       </c>
       <c r="G97" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="H97" s="9" t="s">
-        <v>128</v>
+        <v>46</v>
+      </c>
+      <c r="H97" s="9">
+        <v>20.035643160334502</v>
       </c>
       <c r="I97" s="9"/>
-    </row>
-    <row r="98" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="C98"/>
-      <c r="D98" s="9"/>
-      <c r="F98" s="9"/>
-      <c r="G98" s="9"/>
-      <c r="H98" s="9"/>
+      <c r="L97" s="9"/>
+    </row>
+    <row r="98" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A98" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="B98" t="s">
+        <v>143</v>
+      </c>
+      <c r="C98" t="s">
+        <v>106</v>
+      </c>
+      <c r="D98" s="9">
+        <v>1</v>
+      </c>
+      <c r="E98" t="s">
+        <v>158</v>
+      </c>
+      <c r="F98" s="9">
+        <v>256</v>
+      </c>
+      <c r="G98" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H98" s="27" t="s">
+        <v>140</v>
+      </c>
       <c r="I98" s="9"/>
-    </row>
-    <row r="99" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
-        <v>100</v>
+      <c r="L98" s="9"/>
+    </row>
+    <row r="99" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A99" s="9" t="s">
+        <v>164</v>
       </c>
       <c r="B99" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C99" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D99" s="9">
         <v>1</v>
       </c>
       <c r="E99" t="s">
-        <v>161</v>
-      </c>
-      <c r="F99" s="9" t="s">
-        <v>117</v>
+        <v>158</v>
+      </c>
+      <c r="F99" s="9">
+        <v>256</v>
       </c>
       <c r="G99" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H99" s="9" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="I99" s="9"/>
-    </row>
-    <row r="100" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
-        <v>100</v>
+      <c r="L99" s="9"/>
+    </row>
+    <row r="100" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A100" s="9" t="s">
+        <v>164</v>
       </c>
       <c r="B100" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C100" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D100" s="9">
         <v>1</v>
       </c>
       <c r="E100" t="s">
-        <v>161</v>
-      </c>
-      <c r="F100" s="9" t="s">
-        <v>117</v>
+        <v>158</v>
+      </c>
+      <c r="F100" s="9">
+        <v>256</v>
       </c>
       <c r="G100" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H100" s="9" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="I100" s="9"/>
-    </row>
-    <row r="101" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
-        <v>100</v>
+      <c r="L100" s="9"/>
+    </row>
+    <row r="101" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A101" s="9" t="s">
+        <v>164</v>
       </c>
       <c r="B101" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C101" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D101" s="9">
         <v>1</v>
       </c>
       <c r="E101" t="s">
-        <v>161</v>
-      </c>
-      <c r="F101" s="9" t="s">
-        <v>117</v>
+        <v>158</v>
+      </c>
+      <c r="F101" s="9">
+        <v>256</v>
       </c>
       <c r="G101" s="9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H101" s="9" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="I101" s="9"/>
-    </row>
-    <row r="102" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="L101" s="9"/>
+    </row>
+    <row r="102" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="C102"/>
       <c r="D102" s="9"/>
       <c r="F102" s="9"/>
       <c r="G102" s="9"/>
       <c r="H102" s="9"/>
       <c r="I102" s="9"/>
-    </row>
-    <row r="103" spans="1:9" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="C103"/>
-    </row>
-    <row r="104" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
-        <v>101</v>
+      <c r="L102" s="9"/>
+    </row>
+    <row r="103" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B103" t="s">
+        <v>143</v>
+      </c>
+      <c r="C103" t="s">
+        <v>106</v>
+      </c>
+      <c r="D103" s="9">
+        <v>1</v>
+      </c>
+      <c r="E103" t="s">
+        <v>159</v>
+      </c>
+      <c r="F103" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G103" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="H103" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="I103" s="9"/>
+      <c r="L103" s="9"/>
+    </row>
+    <row r="104" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A104" s="9" t="s">
+        <v>165</v>
       </c>
       <c r="B104" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C104" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D104" s="9">
         <v>1</v>
       </c>
-      <c r="F104" s="23" t="s">
-        <v>133</v>
-      </c>
-      <c r="G104" s="9"/>
-      <c r="H104" s="9"/>
-      <c r="I104" s="23" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
-        <v>102</v>
+      <c r="E104" t="s">
+        <v>159</v>
+      </c>
+      <c r="F104" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G104" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="H104" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="I104" s="9"/>
+      <c r="L104" s="9"/>
+    </row>
+    <row r="105" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A105" s="9" t="s">
+        <v>165</v>
       </c>
       <c r="B105" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C105" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D105" s="9">
         <v>1</v>
       </c>
-      <c r="F105" s="23" t="s">
-        <v>134</v>
-      </c>
-      <c r="G105" s="9"/>
-      <c r="H105" s="9"/>
-      <c r="I105" s="23" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="E105" t="s">
+        <v>159</v>
+      </c>
+      <c r="F105" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G105" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="H105" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="I105" s="9"/>
+      <c r="L105" s="9"/>
+    </row>
+    <row r="106" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="C106"/>
       <c r="D106" s="9"/>
-      <c r="F106" s="23"/>
+      <c r="F106" s="9"/>
       <c r="G106" s="9"/>
       <c r="H106" s="9"/>
-      <c r="I106" s="23"/>
-    </row>
-    <row r="107" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B107" t="s">
-        <v>145</v>
-      </c>
-      <c r="C107" t="s">
-        <v>108</v>
-      </c>
-      <c r="D107" s="9">
-        <v>1</v>
-      </c>
-      <c r="F107" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="G107" s="9"/>
-      <c r="H107" s="9"/>
-      <c r="I107" s="23" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="I106" s="9"/>
+      <c r="L106" s="9"/>
+    </row>
+    <row r="107" spans="1:12" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="C107"/>
+    </row>
+    <row r="108" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B108" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C108" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D108" s="9">
         <v>1</v>
       </c>
+      <c r="E108" t="s">
+        <v>171</v>
+      </c>
       <c r="F108" s="23" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="G108" s="9"/>
       <c r="H108" s="9"/>
       <c r="I108" s="23" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+      <c r="L108" s="9"/>
+    </row>
+    <row r="109" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B109" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C109" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D109" s="9">
         <v>1</v>
       </c>
+      <c r="E109" t="s">
+        <v>172</v>
+      </c>
       <c r="F109" s="23" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="G109" s="9"/>
       <c r="H109" s="9"/>
       <c r="I109" s="23" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B110" t="s">
-        <v>145</v>
-      </c>
-      <c r="C110" t="s">
-        <v>108</v>
-      </c>
-      <c r="D110" s="9">
-        <v>1</v>
-      </c>
-      <c r="F110" s="23" t="s">
-        <v>138</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="L109" s="9"/>
+    </row>
+    <row r="110" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="C110"/>
+      <c r="D110" s="9"/>
+      <c r="F110" s="23"/>
       <c r="G110" s="9"/>
       <c r="H110" s="9"/>
-      <c r="I110" s="23" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C111" s="9"/>
-      <c r="D111" s="9"/>
-      <c r="F111" s="9"/>
+      <c r="I110" s="23"/>
+      <c r="L110" s="9"/>
+    </row>
+    <row r="111" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B111" t="s">
+        <v>143</v>
+      </c>
+      <c r="C111" t="s">
+        <v>106</v>
+      </c>
+      <c r="D111" s="9">
+        <v>1</v>
+      </c>
+      <c r="E111" t="s">
+        <v>173</v>
+      </c>
+      <c r="F111" s="23" t="s">
+        <v>133</v>
+      </c>
       <c r="G111" s="9"/>
       <c r="H111" s="9"/>
-      <c r="I111" s="9"/>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C112" s="9"/>
-      <c r="D112" s="9"/>
-      <c r="F112" s="9"/>
+      <c r="I111" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="L111" s="9"/>
+    </row>
+    <row r="112" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B112" t="s">
+        <v>143</v>
+      </c>
+      <c r="C112" t="s">
+        <v>106</v>
+      </c>
+      <c r="D112" s="9">
+        <v>1</v>
+      </c>
+      <c r="E112" t="s">
+        <v>174</v>
+      </c>
+      <c r="F112" s="23" t="s">
+        <v>134</v>
+      </c>
       <c r="G112" s="9"/>
       <c r="H112" s="9"/>
-      <c r="I112" s="9"/>
-    </row>
-    <row r="113" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C113" s="9"/>
-      <c r="D113" s="9"/>
-      <c r="F113" s="9"/>
+      <c r="I112" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="L112" s="9"/>
+    </row>
+    <row r="113" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B113" t="s">
+        <v>143</v>
+      </c>
+      <c r="C113" t="s">
+        <v>106</v>
+      </c>
+      <c r="D113" s="9">
+        <v>1</v>
+      </c>
+      <c r="E113" t="s">
+        <v>175</v>
+      </c>
+      <c r="F113" s="23" t="s">
+        <v>135</v>
+      </c>
       <c r="G113" s="9"/>
       <c r="H113" s="9"/>
-      <c r="I113" s="9"/>
-    </row>
-    <row r="114" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C114" s="9"/>
-      <c r="D114" s="9"/>
-      <c r="F114" s="9"/>
+      <c r="I113" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="L113" s="9"/>
+    </row>
+    <row r="114" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B114" t="s">
+        <v>143</v>
+      </c>
+      <c r="C114" t="s">
+        <v>106</v>
+      </c>
+      <c r="D114" s="9">
+        <v>1</v>
+      </c>
+      <c r="E114" t="s">
+        <v>176</v>
+      </c>
+      <c r="F114" s="23" t="s">
+        <v>136</v>
+      </c>
       <c r="G114" s="9"/>
       <c r="H114" s="9"/>
-      <c r="I114" s="9"/>
-    </row>
-    <row r="115" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="I114" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="L114" s="9"/>
+    </row>
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C115" s="9"/>
       <c r="D115" s="9"/>
       <c r="F115" s="9"/>
@@ -4271,7 +4477,7 @@
       <c r="H115" s="9"/>
       <c r="I115" s="9"/>
     </row>
-    <row r="116" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C116" s="9"/>
       <c r="D116" s="9"/>
       <c r="F116" s="9"/>
@@ -4279,7 +4485,7 @@
       <c r="H116" s="9"/>
       <c r="I116" s="9"/>
     </row>
-    <row r="117" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C117" s="9"/>
       <c r="D117" s="9"/>
       <c r="F117" s="9"/>
@@ -4287,7 +4493,7 @@
       <c r="H117" s="9"/>
       <c r="I117" s="9"/>
     </row>
-    <row r="118" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C118" s="9"/>
       <c r="D118" s="9"/>
       <c r="F118" s="9"/>
@@ -4295,7 +4501,7 @@
       <c r="H118" s="9"/>
       <c r="I118" s="9"/>
     </row>
-    <row r="119" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C119" s="9"/>
       <c r="D119" s="9"/>
       <c r="F119" s="9"/>
@@ -4303,7 +4509,7 @@
       <c r="H119" s="9"/>
       <c r="I119" s="9"/>
     </row>
-    <row r="120" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C120" s="9"/>
       <c r="D120" s="9"/>
       <c r="F120" s="9"/>
@@ -4311,7 +4517,7 @@
       <c r="H120" s="9"/>
       <c r="I120" s="9"/>
     </row>
-    <row r="121" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C121" s="9"/>
       <c r="D121" s="9"/>
       <c r="F121" s="9"/>
@@ -4319,7 +4525,7 @@
       <c r="H121" s="9"/>
       <c r="I121" s="9"/>
     </row>
-    <row r="122" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C122" s="9"/>
       <c r="D122" s="9"/>
       <c r="F122" s="9"/>
@@ -4327,7 +4533,7 @@
       <c r="H122" s="9"/>
       <c r="I122" s="9"/>
     </row>
-    <row r="123" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C123" s="9"/>
       <c r="D123" s="9"/>
       <c r="F123" s="9"/>
@@ -4335,7 +4541,7 @@
       <c r="H123" s="9"/>
       <c r="I123" s="9"/>
     </row>
-    <row r="124" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C124" s="9"/>
       <c r="D124" s="9"/>
       <c r="F124" s="9"/>
@@ -4343,7 +4549,7 @@
       <c r="H124" s="9"/>
       <c r="I124" s="9"/>
     </row>
-    <row r="125" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C125" s="9"/>
       <c r="D125" s="9"/>
       <c r="F125" s="9"/>
@@ -4351,7 +4557,7 @@
       <c r="H125" s="9"/>
       <c r="I125" s="9"/>
     </row>
-    <row r="126" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C126" s="9"/>
       <c r="D126" s="9"/>
       <c r="F126" s="9"/>
@@ -4359,7 +4565,7 @@
       <c r="H126" s="9"/>
       <c r="I126" s="9"/>
     </row>
-    <row r="127" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C127" s="9"/>
       <c r="D127" s="9"/>
       <c r="F127" s="9"/>
@@ -4367,7 +4573,7 @@
       <c r="H127" s="9"/>
       <c r="I127" s="9"/>
     </row>
-    <row r="128" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C128" s="9"/>
       <c r="D128" s="9"/>
       <c r="F128" s="9"/>
@@ -4759,11 +4965,43 @@
       <c r="H176" s="9"/>
       <c r="I176" s="9"/>
     </row>
+    <row r="177" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C177" s="9"/>
+      <c r="D177" s="9"/>
+      <c r="F177" s="9"/>
+      <c r="G177" s="9"/>
+      <c r="H177" s="9"/>
+      <c r="I177" s="9"/>
+    </row>
+    <row r="178" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C178" s="9"/>
+      <c r="D178" s="9"/>
+      <c r="F178" s="9"/>
+      <c r="G178" s="9"/>
+      <c r="H178" s="9"/>
+      <c r="I178" s="9"/>
+    </row>
+    <row r="179" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C179" s="9"/>
+      <c r="D179" s="9"/>
+      <c r="F179" s="9"/>
+      <c r="G179" s="9"/>
+      <c r="H179" s="9"/>
+      <c r="I179" s="9"/>
+    </row>
+    <row r="180" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C180" s="9"/>
+      <c r="D180" s="9"/>
+      <c r="F180" s="9"/>
+      <c r="G180" s="9"/>
+      <c r="H180" s="9"/>
+      <c r="I180" s="9"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="F23:F24 F99:F101" numberStoredAsText="1"/>
+    <ignoredError sqref="F27:F28 F103:F105" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>